<commit_message>
added venv, removed second entry, added signature and added .exe file
</commit_message>
<xml_diff>
--- a/TOPSIS_sample.xlsx
+++ b/TOPSIS_sample.xlsx
@@ -151,10 +151,10 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:F23"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.45"/>
@@ -303,48 +303,13 @@
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="E23" s="0"/>
-      <c r="F23" s="0"/>
-    </row>
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
modified file selection, added feedback
</commit_message>
<xml_diff>
--- a/TOPSIS_sample.xlsx
+++ b/TOPSIS_sample.xlsx
@@ -148,13 +148,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="9:23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.45"/>
@@ -255,61 +255,6 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
fixed blank cell bug
</commit_message>
<xml_diff>
--- a/TOPSIS_sample.xlsx
+++ b/TOPSIS_sample.xlsx
@@ -151,10 +151,10 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="9:23"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="9:19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.45"/>

</xml_diff>